<commit_message>
design and implementation grammarly
</commit_message>
<xml_diff>
--- a/Report Helper Documents/Testing.xlsx
+++ b/Report Helper Documents/Testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cameronclark/Documents/UCT/EEE4022S/EEE4022S_Salinity_JCP24-03/Report Helper Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CECB1C-BD36-1445-A411-B5F675A3CD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B5DD79-51C8-D44A-93AD-43C0AF3A0F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="5" xr2:uid="{CC746ED0-B61A-5B42-A9B2-4A328CF3FB68}"/>
+    <workbookView xWindow="-28800" yWindow="1940" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{CC746ED0-B61A-5B42-A9B2-4A328CF3FB68}"/>
   </bookViews>
   <sheets>
     <sheet name="DAC Range" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="244">
   <si>
     <t>VDD</t>
   </si>
@@ -784,6 +784,18 @@
   <si>
     <t>0,0,0,3;156,0,0,2;307,0,0,2;446,0,0,2;568,0,0,2;668,0,0,3;743,0,0,20;789,0,0,161;804,0,0,327;789,0,0,489;743,0,0,644;669,0,0,780;569,0,0,890;447,0,0,971;308,0,0,1028;157,0,0,1047;0,0,0,-2;-156,0,0,-2;-307,0,0,-2;-446,0,0,-2;-568,0,0,-2;-668,0,0,-2;-743,0,0,-2;-789,0,0,-5;-804,0,0,-124;-789,0,0,-302;-743,0,0,-468;-669,0,0,-611;-569,0,0,-730;-447,0,0,-824;-308,0,0,-885;-157,0,0,-915;0,0,0,2;156,0,0,1;307,0,0,1;446,0,0,2;568,0,0,1;668,0,0,2;743,0,0,3;789,0,0,41;804,0,0,204;789,0,0,372;743,0,0,531;669,0,0,670;569,0,0,787;447,0,0,873;308,0,0,931;157,0,0,956;0,0,0,-1;-156,0,0,-2;-307,0,0,-2;-446,0,0,-2;-568,0,0,-2;-668,0,0,-2;-743,0,0,-4;-789,0,0,-32;-804,0,0,-192;-789,0,0,-370;-743,0,0,-529;-669,0,0,-666;-569,0,0,-789;-447,0,0,-881;-308,0,0,-941;-157,0,0,-969;0,0,0,2;156,0,0,2;307,0,0,2;446,0,0,2;568,0,0,2;668,0,0,2;743,0,0,2;789,0,0,14;804,0,0,159;789,0,0,328;743,0,0,490;669,0,0,630;569,0,0,748;447,0,0,837;308,0,0,896;157,0,0,925;0,0,0,-1;-156,0,0,-2;-307,0,0,-2;-446,0,0,-2;-568,0,0,-2;-668,0,0,-2;-743,0,0,-4;-789,0,0,-52;-804,0,0,-222;-789,0,0,-394;-743,0,0,-556;-669,0,0,-699;-569,0,0,-817;-447,0,0,-906;-308,0,0,-968;-157,0,0,-995;0,0,0,2;156,0,0,1;307,0,0,2;446,0,0,1;568,0,0,2;668,0,0,2;743,0,0,3;789,0,0,6;804,0,0,137;789,0,0,309;743,0,0,468;669,0,0,609;569,0,0,724;447,0,0,817;308,0,0,874;157,0,0,900;0,0,0,-2;-156,0,0,-2;-307,0,0,-2;-446,0,0,-3;-568,0,0,-2;-668,0,0,-7;-743,0,0,-4;-789,0,0,-75;-804,0,0,-241;-789,0,0,-414;-743,0,0,-574;-669,0,0,-718;-569,0,0,-835;-447,0,0,-926;-308,0,0,-980;-157,0,0,-1014;</t>
   </si>
+  <si>
+    <t>150,596,348,759;182,724,421,970;215,855,496,1185;248,987,571,1395;281,1119,645,1600;314,1251,721,1785;346,1379,793,1947;379,1510,868,2127;412,1642,943,2315;445,1774,1018,2485;478,1906,1094,2675;510,2033,1167,2846;543,2165,1241,3028;576,2297,1317,3345;609,2428,1392,3401;642,2561,1467,3751;674,2689,1540,3750;707,2820,1614,3856;740,2952,1689,3935;773,3084,1764,4011;</t>
+  </si>
+  <si>
+    <t>150,596,348,955;182,723,421,1130;215,855,496,1322;248,986,571,1502;281,1119,646,1656;314,1251,721,1827;346,1379,794,1999;379,1510,869,2182;412,1642,945,2421;445,1774,1020,2536;478,1905,1095,2742;510,2033,1168,2879;543,2165,1242,3061;576,2297,1319,3243;609,2429,1394,3447;642,2561,1468,3553;674,2689,1542,3710;707,2821,1616,3840;740,2952,1691,3929;773,3085,1767,4004;</t>
+  </si>
+  <si>
+    <t>150,596,349,939;182,724,422,1114;215,855,496,1311;248,987,572,1487;281,1119,646,1669;314,1251,722,1843;346,1379,795,2020;379,1511,870,2197;412,1642,944,2381;445,1774,1019,2555;478,1905,1095,2741;510,2033,1168,2919;543,2165,1243,3100;576,2297,1318,3261;609,2429,1393,3422;642,2561,1468,3601;674,2689,1542,3754;707,2821,1617,3879;740,2952,1692,3957;773,3085,1767,4019;</t>
+  </si>
+  <si>
+    <t>150,596,348,1030;182,724,421,1208;215,855,496,1389;248,987,571,1560;281,1119,646,1732;314,1251,721,1918;346,1379,794,2077;379,1510,869,2258;412,1642,944,2423;445,1773,1019,2597;478,1905,1094,2773;510,2033,1167,2949;543,2166,1241,3136;576,2297,1317,3313;609,2429,1392,3491;642,2561,1467,3660;674,2688,1540,3799;707,2821,1615,3894;740,2952,1689,3973;773,3085,1764,4026;</t>
+  </si>
 </sst>
 </file>
 
@@ -5390,10 +5402,10 @@
                   <c:v>0.48029304029304026</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.58344322344322341</c:v>
+                  <c:v>0.58263736263736265</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.68981684981684976</c:v>
+                  <c:v>0.68901098901098901</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.79538461538461536</c:v>
@@ -5408,7 +5420,7 @@
                   <c:v>1.1112820512820512</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.2176556776556777</c:v>
+                  <c:v>1.2168498168498167</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1.3232234432234431</c:v>
@@ -5429,22 +5441,22 @@
                   <c:v>1.8510622710622708</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.9574358974358974</c:v>
+                  <c:v>1.9566300366300367</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>2.0638095238095238</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.1669597069597066</c:v>
+                  <c:v>2.1661538461538461</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>2.273333333333333</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.3797069597069598</c:v>
+                  <c:v>2.3789010989010988</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.4860805860805861</c:v>
+                  <c:v>2.4852747252747251</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -6896,7 +6908,7 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="500"/>
                 <c:pt idx="0">
-                  <c:v>0.28124542124542123</c:v>
+                  <c:v>0.28043956043956042</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.33926739926739924</c:v>
@@ -6908,7 +6920,7 @@
                   <c:v>0.46014652014652013</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.52058608058608047</c:v>
+                  <c:v>0.51978021978021982</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.58102564102564092</c:v>
@@ -6926,7 +6938,7 @@
                   <c:v>0.82036630036630032</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.88161172161172152</c:v>
+                  <c:v>0.88241758241758239</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0.94043956043956045</c:v>
@@ -6935,25 +6947,25 @@
                   <c:v>1.0008791208791208</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.062124542124542</c:v>
+                  <c:v>1.0613186813186812</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.1225641025641024</c:v>
+                  <c:v>1.1217582417582417</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.1838095238095239</c:v>
+                  <c:v>1.1821978021978021</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.2434432234432233</c:v>
+                  <c:v>1.2410256410256411</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.303076923076923</c:v>
+                  <c:v>1.3006593406593405</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.3635164835164835</c:v>
+                  <c:v>1.361098901098901</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.4239560439560439</c:v>
+                  <c:v>1.4215384615384614</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -8828,10 +8840,10 @@
                   <c:v>0.48029304029304026</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.58344322344322341</c:v>
+                  <c:v>0.58263736263736265</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.68981684981684976</c:v>
+                  <c:v>0.68901098901098901</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.79538461538461536</c:v>
@@ -8846,7 +8858,7 @@
                   <c:v>1.1112820512820512</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.2176556776556777</c:v>
+                  <c:v>1.2168498168498167</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1.3232234432234431</c:v>
@@ -8867,22 +8879,22 @@
                   <c:v>1.8510622710622708</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.9574358974358974</c:v>
+                  <c:v>1.9566300366300367</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>2.0638095238095238</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.1669597069597066</c:v>
+                  <c:v>2.1661538461538461</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>2.273333333333333</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.3797069597069598</c:v>
+                  <c:v>2.3789010989010988</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.4860805860805861</c:v>
+                  <c:v>2.4852747252747251</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -10334,64 +10346,64 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="500"/>
                 <c:pt idx="0">
-                  <c:v>0.94688644688644685</c:v>
+                  <c:v>0.79699633699633698</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1410989010989012</c:v>
+                  <c:v>0.98717948717948723</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3393406593406592</c:v>
+                  <c:v>1.1789743589743589</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5383882783882783</c:v>
+                  <c:v>1.3675457875457875</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.7358241758241757</c:v>
+                  <c:v>1.5545054945054944</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.9324542124542123</c:v>
+                  <c:v>1.7414652014652012</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.121025641025641</c:v>
+                  <c:v>1.9243956043956043</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.2886446886446885</c:v>
+                  <c:v>2.1186080586080585</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.4046886446886444</c:v>
+                  <c:v>2.2934798534798535</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.4917216117216112</c:v>
+                  <c:v>2.4764102564102561</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.5537728937728934</c:v>
+                  <c:v>2.6319413919413917</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.610989010989011</c:v>
+                  <c:v>2.7495970695970691</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.6778754578754578</c:v>
+                  <c:v>2.8446886446886448</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.735091575091575</c:v>
+                  <c:v>2.9252747252747251</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.8003663003663002</c:v>
+                  <c:v>2.9832967032967028</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.8640293040293039</c:v>
+                  <c:v>3.0308424908424905</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.9293040293040291</c:v>
+                  <c:v>3.0791941391941391</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.9695970695970697</c:v>
+                  <c:v>3.1049816849816847</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.0211721611721609</c:v>
+                  <c:v>3.1404395604395603</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.059047619047619</c:v>
+                  <c:v>3.1621978021978019</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -12262,7 +12274,7 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="500"/>
                 <c:pt idx="0">
-                  <c:v>0.28124542124542123</c:v>
+                  <c:v>0.28043956043956042</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.33926739926739924</c:v>
@@ -12274,7 +12286,7 @@
                   <c:v>0.46014652014652013</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.52058608058608047</c:v>
+                  <c:v>0.51978021978021982</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.58102564102564092</c:v>
@@ -12292,7 +12304,7 @@
                   <c:v>0.82036630036630032</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.88161172161172152</c:v>
+                  <c:v>0.88241758241758239</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0.94043956043956045</c:v>
@@ -12301,25 +12313,25 @@
                   <c:v>1.0008791208791208</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.062124542124542</c:v>
+                  <c:v>1.0613186813186812</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.1225641025641024</c:v>
+                  <c:v>1.1217582417582417</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.1838095238095239</c:v>
+                  <c:v>1.1821978021978021</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.2434432234432233</c:v>
+                  <c:v>1.2410256410256411</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.303076923076923</c:v>
+                  <c:v>1.3006593406593405</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.3635164835164835</c:v>
+                  <c:v>1.361098901098901</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.4239560439560439</c:v>
+                  <c:v>1.4215384615384614</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -13771,64 +13783,64 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="500"/>
                 <c:pt idx="0">
-                  <c:v>0.94688644688644685</c:v>
+                  <c:v>0.79699633699633698</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1410989010989012</c:v>
+                  <c:v>0.98717948717948723</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3393406593406592</c:v>
+                  <c:v>1.1789743589743589</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5383882783882783</c:v>
+                  <c:v>1.3675457875457875</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.7358241758241757</c:v>
+                  <c:v>1.5545054945054944</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.9324542124542123</c:v>
+                  <c:v>1.7414652014652012</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.121025641025641</c:v>
+                  <c:v>1.9243956043956043</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.2886446886446885</c:v>
+                  <c:v>2.1186080586080585</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.4046886446886444</c:v>
+                  <c:v>2.2934798534798535</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.4917216117216112</c:v>
+                  <c:v>2.4764102564102561</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.5537728937728934</c:v>
+                  <c:v>2.6319413919413917</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.610989010989011</c:v>
+                  <c:v>2.7495970695970691</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.6778754578754578</c:v>
+                  <c:v>2.8446886446886448</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.735091575091575</c:v>
+                  <c:v>2.9252747252747251</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.8003663003663002</c:v>
+                  <c:v>2.9832967032967028</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.8640293040293039</c:v>
+                  <c:v>3.0308424908424905</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.9293040293040291</c:v>
+                  <c:v>3.0791941391941391</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.9695970695970697</c:v>
+                  <c:v>3.1049816849816847</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.0211721611721609</c:v>
+                  <c:v>3.1404395604395603</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.059047619047619</c:v>
+                  <c:v>3.1621978021978019</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -15673,10 +15685,10 @@
                   <c:v>0.48029304029304026</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.58344322344322341</c:v>
+                  <c:v>0.58263736263736265</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.68981684981684976</c:v>
+                  <c:v>0.68901098901098901</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.79538461538461536</c:v>
@@ -15691,7 +15703,7 @@
                   <c:v>1.1112820512820512</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.2176556776556777</c:v>
+                  <c:v>1.2168498168498167</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1.3232234432234431</c:v>
@@ -15712,22 +15724,22 @@
                   <c:v>1.8510622710622708</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.9574358974358974</c:v>
+                  <c:v>1.9566300366300367</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>2.0638095238095238</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.1669597069597066</c:v>
+                  <c:v>2.1661538461538461</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>2.273333333333333</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.3797069597069598</c:v>
+                  <c:v>2.3789010989010988</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.4860805860805861</c:v>
+                  <c:v>2.4852747252747251</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -17179,64 +17191,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="500"/>
                 <c:pt idx="0">
-                  <c:v>3.36676217765043</c:v>
+                  <c:v>2.8419540229885061</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.3634204275534447</c:v>
+                  <c:v>2.909738717339668</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.350806451612903</c:v>
+                  <c:v>2.9495967741935485</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.3432574430823117</c:v>
+                  <c:v>2.9719789842381785</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.3343653250773997</c:v>
+                  <c:v>2.990697674418604</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.3259361997226078</c:v>
+                  <c:v>2.9972260748959778</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.3148614609571787</c:v>
+                  <c:v>3.0075566750629723</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.2681242807825086</c:v>
+                  <c:v>3.0253164556962022</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.1610169491525419</c:v>
+                  <c:v>3.0148305084745761</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.0373280943025538</c:v>
+                  <c:v>3.0186640471512769</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.8967093235831807</c:v>
+                  <c:v>2.9826484018264838</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.7763496143958868</c:v>
+                  <c:v>2.9237360754070258</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.6755233494363933</c:v>
+                  <c:v>2.8421900161030598</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.575113808801214</c:v>
+                  <c:v>2.7562642369020502</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.494615936826992</c:v>
+                  <c:v>2.6594827586206895</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.4193328795098705</c:v>
+                  <c:v>2.5637355146557601</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.355800388852884</c:v>
+                  <c:v>2.4811688311688309</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.2789115646258504</c:v>
+                  <c:v>2.3872366790582404</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.2157210401891252</c:v>
+                  <c:v>2.3072824156305507</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.1482739105829087</c:v>
+                  <c:v>2.2244897959183674</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -26629,14 +26641,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FAF9EF3-1AC3-AC4D-852C-E437797668DB}">
   <dimension ref="A1:AC1048576"/>
   <sheetViews>
-    <sheetView zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:J3"/>
+    <sheetView tabSelected="1" zoomScale="41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA46" sqref="AA46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" customWidth="1"/>
     <col min="17" max="17" width="13" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="12.5" bestFit="1" customWidth="1"/>
@@ -26742,8 +26755,8 @@
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="str">
-        <f>AC101</f>
-        <v>150,596,349,1175;182,724,421,1416;215,856,496,1662;248,987,571,1909;281,1119,646,2154;314,1251,721,2398;346,1379,794,2632;379,1511,869,2840;412,1642,944,2984;445,1773,1018,3092;478,1905,1094,3169;510,2033,1167,3240;543,2165,1242,3323;576,2297,1318,3394;609,2429,1393,3475;642,2561,1469,3554;674,2689,1543,3635;707,2821,1617,3685;740,2953,1692,3749;773,3085,1767,3796;</v>
+        <f>AC69</f>
+        <v>150,596,348,989;182,723,421,1225;215,855,496,1463;248,987,571,1697;281,1119,645,1929;314,1251,721,2161;346,1379,794,2388;379,1510,869,2629;412,1642,944,2846;445,1773,1018,3073;478,1905,1095,3266;510,2033,1167,3412;543,2165,1242,3530;576,2297,1317,3630;609,2428,1392,3702;642,2561,1467,3761;674,2688,1540,3821;707,2821,1614,3853;740,2952,1689,3897;773,3084,1764,3924;</v>
       </c>
       <c r="B3" t="str" cm="1">
         <f t="array" ref="B3:E22">_xlfn.TEXTSPLIT(A3,",",";",TRUE)</f>
@@ -26753,10 +26766,10 @@
         <v>596</v>
       </c>
       <c r="D3" t="str">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E3" t="str">
-        <v>1175</v>
+        <v>989</v>
       </c>
       <c r="F3" s="4">
         <f>B3*3.3/1023</f>
@@ -26768,15 +26781,15 @@
       </c>
       <c r="H3" s="6">
         <f>D3*3.3/4095</f>
-        <v>0.28124542124542123</v>
+        <v>0.28043956043956042</v>
       </c>
       <c r="I3" s="6">
         <f>E3*3.3/4095</f>
-        <v>0.94688644688644685</v>
+        <v>0.79699633699633698</v>
       </c>
       <c r="J3">
         <f>I3/H3</f>
-        <v>3.36676217765043</v>
+        <v>2.8419540229885061</v>
       </c>
       <c r="Q3" t="s">
         <v>50</v>
@@ -26817,13 +26830,13 @@
         <v>182</v>
       </c>
       <c r="C4" t="str">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D4" t="str">
         <v>421</v>
       </c>
       <c r="E4" t="str">
-        <v>1416</v>
+        <v>1225</v>
       </c>
       <c r="F4" s="4">
         <f t="shared" ref="F4:F52" si="0">B4*3.3/1023</f>
@@ -26831,7 +26844,7 @@
       </c>
       <c r="G4" s="4">
         <f t="shared" ref="G4:G43" si="1">C4*3.3/4095</f>
-        <v>0.58344322344322341</v>
+        <v>0.58263736263736265</v>
       </c>
       <c r="H4" s="6">
         <f t="shared" ref="H4:H67" si="2">D4*3.3/4095</f>
@@ -26839,11 +26852,11 @@
       </c>
       <c r="I4" s="6">
         <f t="shared" ref="I4:I67" si="3">E4*3.3/4095</f>
-        <v>1.1410989010989012</v>
+        <v>0.98717948717948723</v>
       </c>
       <c r="J4">
         <f t="shared" ref="J4:J67" si="4">I4/H4</f>
-        <v>3.3634204275534447</v>
+        <v>2.909738717339668</v>
       </c>
       <c r="Q4" t="s">
         <v>49</v>
@@ -26884,13 +26897,13 @@
         <v>215</v>
       </c>
       <c r="C5" t="str">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="D5" t="str">
         <v>496</v>
       </c>
       <c r="E5" t="str">
-        <v>1662</v>
+        <v>1463</v>
       </c>
       <c r="F5" s="4">
         <f t="shared" si="0"/>
@@ -26898,7 +26911,7 @@
       </c>
       <c r="G5" s="4">
         <f t="shared" si="1"/>
-        <v>0.68981684981684976</v>
+        <v>0.68901098901098901</v>
       </c>
       <c r="H5" s="6">
         <f t="shared" si="2"/>
@@ -26906,11 +26919,11 @@
       </c>
       <c r="I5" s="6">
         <f t="shared" si="3"/>
-        <v>1.3393406593406592</v>
+        <v>1.1789743589743589</v>
       </c>
       <c r="J5">
         <f t="shared" si="4"/>
-        <v>3.350806451612903</v>
+        <v>2.9495967741935485</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.2">
@@ -26924,7 +26937,7 @@
         <v>571</v>
       </c>
       <c r="E6" t="str">
-        <v>1909</v>
+        <v>1697</v>
       </c>
       <c r="F6" s="4">
         <f t="shared" si="0"/>
@@ -26940,11 +26953,11 @@
       </c>
       <c r="I6" s="6">
         <f t="shared" si="3"/>
-        <v>1.5383882783882783</v>
+        <v>1.3675457875457875</v>
       </c>
       <c r="J6">
         <f t="shared" si="4"/>
-        <v>3.3432574430823117</v>
+        <v>2.9719789842381785</v>
       </c>
       <c r="Q6" t="s">
         <v>47</v>
@@ -26988,10 +27001,10 @@
         <v>1119</v>
       </c>
       <c r="D7" t="str">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="E7" t="str">
-        <v>2154</v>
+        <v>1929</v>
       </c>
       <c r="F7" s="4">
         <f t="shared" si="0"/>
@@ -27003,15 +27016,15 @@
       </c>
       <c r="H7" s="6">
         <f t="shared" si="2"/>
-        <v>0.52058608058608047</v>
+        <v>0.51978021978021982</v>
       </c>
       <c r="I7" s="6">
         <f t="shared" si="3"/>
-        <v>1.7358241758241757</v>
+        <v>1.5545054945054944</v>
       </c>
       <c r="J7">
         <f t="shared" si="4"/>
-        <v>3.3343653250773997</v>
+        <v>2.990697674418604</v>
       </c>
       <c r="Q7" t="s">
         <v>48</v>
@@ -27058,7 +27071,7 @@
         <v>721</v>
       </c>
       <c r="E8" t="str">
-        <v>2398</v>
+        <v>2161</v>
       </c>
       <c r="F8" s="4">
         <f t="shared" si="0"/>
@@ -27074,11 +27087,11 @@
       </c>
       <c r="I8" s="6">
         <f t="shared" si="3"/>
-        <v>1.9324542124542123</v>
+        <v>1.7414652014652012</v>
       </c>
       <c r="J8">
         <f t="shared" si="4"/>
-        <v>3.3259361997226078</v>
+        <v>2.9972260748959778</v>
       </c>
       <c r="AC8" s="2"/>
     </row>
@@ -27093,7 +27106,7 @@
         <v>794</v>
       </c>
       <c r="E9" t="str">
-        <v>2632</v>
+        <v>2388</v>
       </c>
       <c r="F9" s="4">
         <f t="shared" si="0"/>
@@ -27109,11 +27122,11 @@
       </c>
       <c r="I9" s="6">
         <f t="shared" si="3"/>
-        <v>2.121025641025641</v>
+        <v>1.9243956043956043</v>
       </c>
       <c r="J9">
         <f t="shared" si="4"/>
-        <v>3.3148614609571787</v>
+        <v>3.0075566750629723</v>
       </c>
       <c r="Q9" t="s">
         <v>57</v>
@@ -27154,13 +27167,13 @@
         <v>379</v>
       </c>
       <c r="C10" t="str">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="D10" t="str">
         <v>869</v>
       </c>
       <c r="E10" t="str">
-        <v>2840</v>
+        <v>2629</v>
       </c>
       <c r="F10" s="4">
         <f t="shared" si="0"/>
@@ -27168,7 +27181,7 @@
       </c>
       <c r="G10" s="4">
         <f t="shared" si="1"/>
-        <v>1.2176556776556777</v>
+        <v>1.2168498168498167</v>
       </c>
       <c r="H10" s="6">
         <f t="shared" si="2"/>
@@ -27176,11 +27189,11 @@
       </c>
       <c r="I10" s="6">
         <f t="shared" si="3"/>
-        <v>2.2886446886446885</v>
+        <v>2.1186080586080585</v>
       </c>
       <c r="J10">
         <f t="shared" si="4"/>
-        <v>3.2681242807825086</v>
+        <v>3.0253164556962022</v>
       </c>
       <c r="Q10" t="s">
         <v>59</v>
@@ -27227,7 +27240,7 @@
         <v>944</v>
       </c>
       <c r="E11" t="str">
-        <v>2984</v>
+        <v>2846</v>
       </c>
       <c r="F11" s="4">
         <f t="shared" si="0"/>
@@ -27243,11 +27256,11 @@
       </c>
       <c r="I11" s="6">
         <f t="shared" si="3"/>
-        <v>2.4046886446886444</v>
+        <v>2.2934798534798535</v>
       </c>
       <c r="J11">
         <f t="shared" si="4"/>
-        <v>3.1610169491525419</v>
+        <v>3.0148305084745761</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.2">
@@ -27261,7 +27274,7 @@
         <v>1018</v>
       </c>
       <c r="E12" t="str">
-        <v>3092</v>
+        <v>3073</v>
       </c>
       <c r="F12" s="4">
         <f t="shared" si="0"/>
@@ -27277,11 +27290,11 @@
       </c>
       <c r="I12" s="6">
         <f t="shared" si="3"/>
-        <v>2.4917216117216112</v>
+        <v>2.4764102564102561</v>
       </c>
       <c r="J12">
         <f t="shared" si="4"/>
-        <v>3.0373280943025538</v>
+        <v>3.0186640471512769</v>
       </c>
       <c r="Q12" t="s">
         <v>61</v>
@@ -27328,10 +27341,10 @@
         <v>1905</v>
       </c>
       <c r="D13" t="str">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="E13" t="str">
-        <v>3169</v>
+        <v>3266</v>
       </c>
       <c r="F13" s="4">
         <f t="shared" si="0"/>
@@ -27343,15 +27356,15 @@
       </c>
       <c r="H13" s="6">
         <f t="shared" si="2"/>
-        <v>0.88161172161172152</v>
+        <v>0.88241758241758239</v>
       </c>
       <c r="I13" s="6">
         <f t="shared" si="3"/>
-        <v>2.5537728937728934</v>
+        <v>2.6319413919413917</v>
       </c>
       <c r="J13">
         <f t="shared" si="4"/>
-        <v>2.8967093235831807</v>
+        <v>2.9826484018264838</v>
       </c>
       <c r="Q13" t="s">
         <v>62</v>
@@ -27401,7 +27414,7 @@
         <v>1167</v>
       </c>
       <c r="E14" t="str">
-        <v>3240</v>
+        <v>3412</v>
       </c>
       <c r="F14" s="4">
         <f t="shared" si="0"/>
@@ -27417,11 +27430,11 @@
       </c>
       <c r="I14" s="6">
         <f t="shared" si="3"/>
-        <v>2.610989010989011</v>
+        <v>2.7495970695970691</v>
       </c>
       <c r="J14">
         <f t="shared" si="4"/>
-        <v>2.7763496143958868</v>
+        <v>2.9237360754070258</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.2">
@@ -27435,7 +27448,7 @@
         <v>1242</v>
       </c>
       <c r="E15" t="str">
-        <v>3323</v>
+        <v>3530</v>
       </c>
       <c r="F15" s="4">
         <f t="shared" si="0"/>
@@ -27451,11 +27464,11 @@
       </c>
       <c r="I15" s="6">
         <f t="shared" si="3"/>
-        <v>2.6778754578754578</v>
+        <v>2.8446886446886448</v>
       </c>
       <c r="J15">
         <f t="shared" si="4"/>
-        <v>2.6755233494363933</v>
+        <v>2.8421900161030598</v>
       </c>
       <c r="Q15" t="s">
         <v>67</v>
@@ -27502,10 +27515,10 @@
         <v>2297</v>
       </c>
       <c r="D16" t="str">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="E16" t="str">
-        <v>3394</v>
+        <v>3630</v>
       </c>
       <c r="F16" s="4">
         <f t="shared" si="0"/>
@@ -27517,15 +27530,15 @@
       </c>
       <c r="H16" s="6">
         <f t="shared" si="2"/>
-        <v>1.062124542124542</v>
+        <v>1.0613186813186812</v>
       </c>
       <c r="I16" s="6">
         <f t="shared" si="3"/>
-        <v>2.735091575091575</v>
+        <v>2.9252747252747251</v>
       </c>
       <c r="J16">
         <f t="shared" si="4"/>
-        <v>2.575113808801214</v>
+        <v>2.7562642369020502</v>
       </c>
       <c r="Q16" t="s">
         <v>68</v>
@@ -27569,13 +27582,13 @@
         <v>609</v>
       </c>
       <c r="C17" t="str">
-        <v>2429</v>
+        <v>2428</v>
       </c>
       <c r="D17" t="str">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="E17" t="str">
-        <v>3475</v>
+        <v>3702</v>
       </c>
       <c r="F17" s="4">
         <f t="shared" si="0"/>
@@ -27583,19 +27596,19 @@
       </c>
       <c r="G17" s="4">
         <f t="shared" si="1"/>
-        <v>1.9574358974358974</v>
+        <v>1.9566300366300367</v>
       </c>
       <c r="H17" s="6">
         <f t="shared" si="2"/>
-        <v>1.1225641025641024</v>
+        <v>1.1217582417582417</v>
       </c>
       <c r="I17" s="6">
         <f t="shared" si="3"/>
-        <v>2.8003663003663002</v>
+        <v>2.9832967032967028</v>
       </c>
       <c r="J17">
         <f t="shared" si="4"/>
-        <v>2.494615936826992</v>
+        <v>2.6594827586206895</v>
       </c>
     </row>
     <row r="18" spans="2:29" x14ac:dyDescent="0.2">
@@ -27606,10 +27619,10 @@
         <v>2561</v>
       </c>
       <c r="D18" t="str">
-        <v>1469</v>
+        <v>1467</v>
       </c>
       <c r="E18" t="str">
-        <v>3554</v>
+        <v>3761</v>
       </c>
       <c r="F18" s="4">
         <f t="shared" si="0"/>
@@ -27621,15 +27634,15 @@
       </c>
       <c r="H18" s="6">
         <f t="shared" si="2"/>
-        <v>1.1838095238095239</v>
+        <v>1.1821978021978021</v>
       </c>
       <c r="I18" s="6">
         <f t="shared" si="3"/>
-        <v>2.8640293040293039</v>
+        <v>3.0308424908424905</v>
       </c>
       <c r="J18">
         <f t="shared" si="4"/>
-        <v>2.4193328795098705</v>
+        <v>2.5637355146557601</v>
       </c>
       <c r="Q18" t="s">
         <v>71</v>
@@ -27673,13 +27686,13 @@
         <v>674</v>
       </c>
       <c r="C19" t="str">
-        <v>2689</v>
+        <v>2688</v>
       </c>
       <c r="D19" t="str">
-        <v>1543</v>
+        <v>1540</v>
       </c>
       <c r="E19" t="str">
-        <v>3635</v>
+        <v>3821</v>
       </c>
       <c r="F19" s="4">
         <f t="shared" si="0"/>
@@ -27687,19 +27700,19 @@
       </c>
       <c r="G19" s="4">
         <f t="shared" si="1"/>
-        <v>2.1669597069597066</v>
+        <v>2.1661538461538461</v>
       </c>
       <c r="H19" s="6">
         <f t="shared" si="2"/>
-        <v>1.2434432234432233</v>
+        <v>1.2410256410256411</v>
       </c>
       <c r="I19" s="6">
         <f t="shared" si="3"/>
-        <v>2.9293040293040291</v>
+        <v>3.0791941391941391</v>
       </c>
       <c r="J19">
         <f t="shared" si="4"/>
-        <v>2.355800388852884</v>
+        <v>2.4811688311688309</v>
       </c>
       <c r="Q19" t="s">
         <v>72</v>
@@ -27746,10 +27759,10 @@
         <v>2821</v>
       </c>
       <c r="D20" t="str">
-        <v>1617</v>
+        <v>1614</v>
       </c>
       <c r="E20" t="str">
-        <v>3685</v>
+        <v>3853</v>
       </c>
       <c r="F20" s="4">
         <f t="shared" si="0"/>
@@ -27761,15 +27774,15 @@
       </c>
       <c r="H20" s="6">
         <f t="shared" si="2"/>
-        <v>1.303076923076923</v>
+        <v>1.3006593406593405</v>
       </c>
       <c r="I20" s="6">
         <f t="shared" si="3"/>
-        <v>2.9695970695970697</v>
+        <v>3.1049816849816847</v>
       </c>
       <c r="J20">
         <f t="shared" si="4"/>
-        <v>2.2789115646258504</v>
+        <v>2.3872366790582404</v>
       </c>
     </row>
     <row r="21" spans="2:29" x14ac:dyDescent="0.2">
@@ -27777,13 +27790,13 @@
         <v>740</v>
       </c>
       <c r="C21" t="str">
-        <v>2953</v>
+        <v>2952</v>
       </c>
       <c r="D21" t="str">
-        <v>1692</v>
+        <v>1689</v>
       </c>
       <c r="E21" t="str">
-        <v>3749</v>
+        <v>3897</v>
       </c>
       <c r="F21" s="4">
         <f t="shared" si="0"/>
@@ -27791,19 +27804,19 @@
       </c>
       <c r="G21" s="4">
         <f t="shared" si="1"/>
-        <v>2.3797069597069598</v>
+        <v>2.3789010989010988</v>
       </c>
       <c r="H21" s="6">
         <f t="shared" si="2"/>
-        <v>1.3635164835164835</v>
+        <v>1.361098901098901</v>
       </c>
       <c r="I21" s="6">
         <f t="shared" si="3"/>
-        <v>3.0211721611721609</v>
+        <v>3.1404395604395603</v>
       </c>
       <c r="J21">
         <f t="shared" si="4"/>
-        <v>2.2157210401891252</v>
+        <v>2.3072824156305507</v>
       </c>
       <c r="Q21" t="s">
         <v>75</v>
@@ -27847,13 +27860,13 @@
         <v>773</v>
       </c>
       <c r="C22" t="str">
-        <v>3085</v>
+        <v>3084</v>
       </c>
       <c r="D22" t="str">
-        <v>1767</v>
+        <v>1764</v>
       </c>
       <c r="E22" t="str">
-        <v>3796</v>
+        <v>3924</v>
       </c>
       <c r="F22" s="4">
         <f t="shared" si="0"/>
@@ -27861,19 +27874,19 @@
       </c>
       <c r="G22" s="4">
         <f t="shared" si="1"/>
-        <v>2.4860805860805861</v>
+        <v>2.4852747252747251</v>
       </c>
       <c r="H22" s="6">
         <f t="shared" si="2"/>
-        <v>1.4239560439560439</v>
+        <v>1.4215384615384614</v>
       </c>
       <c r="I22" s="6">
         <f t="shared" si="3"/>
-        <v>3.059047619047619</v>
+        <v>3.1621978021978019</v>
       </c>
       <c r="J22">
         <f t="shared" si="4"/>
-        <v>2.1482739105829087</v>
+        <v>2.2244897959183674</v>
       </c>
       <c r="Q22" t="s">
         <v>76</v>
@@ -29747,7 +29760,7 @@
       </c>
       <c r="L58" t="str">
         <f>SUBSTITUTE(_xlfn.TEXTJOIN(" ",TRUE,G3:G22),",",".")</f>
-        <v>0.48029304029304 0.583443223443223 0.68981684981685 0.795384615384615 0.901758241758242 1.00813186813187 1.11128205128205 1.21765567765568 1.32322344322344 1.42879120879121 1.53516483516484 1.63831501831502 1.74468864468864 1.85106227106227 1.9574358974359 2.06380952380952 2.16695970695971 2.27333333333333 2.37970695970696 2.48608058608059</v>
+        <v>0.48029304029304 0.582637362637363 0.689010989010989 0.795384615384615 0.901758241758242 1.00813186813187 1.11128205128205 1.21684981684982 1.32322344322344 1.42879120879121 1.53516483516484 1.63831501831502 1.74468864468864 1.85106227106227 1.95663003663004 2.06380952380952 2.16615384615385 2.27333333333333 2.3789010989011 2.48527472527473</v>
       </c>
       <c r="Q58" t="s">
         <v>151</v>
@@ -29812,7 +29825,7 @@
       </c>
       <c r="L59" t="str">
         <f>SUBSTITUTE(_xlfn.TEXTJOIN(" ",TRUE,I3:I22),",",".")</f>
-        <v>0.946886446886447 1.1410989010989 1.33934065934066 1.53838827838828 1.73582417582418 1.93245421245421 2.12102564102564 2.28864468864469 2.40468864468864 2.49172161172161 2.55377289377289 2.61098901098901 2.67787545787546 2.73509157509157 2.8003663003663 2.8640293040293 2.92930402930403 2.96959706959707 3.02117216117216 3.05904761904762</v>
+        <v>0.796996336996337 0.987179487179487 1.17897435897436 1.36754578754579 1.55450549450549 1.7414652014652 1.9243956043956 2.11860805860806 2.29347985347985 2.47641025641026 2.63194139194139 2.74959706959707 2.84468864468864 2.92527472527473 2.9832967032967 3.03084249084249 3.07919413919414 3.10498168498168 3.14043956043956 3.1621978021978</v>
       </c>
       <c r="Q59" t="s">
         <v>152</v>
@@ -29877,7 +29890,7 @@
       </c>
       <c r="L60" t="str">
         <f>SUBSTITUTE(_xlfn.TEXTJOIN(" ",TRUE,J3:J22),",",".")</f>
-        <v>3.36676217765043 3.36342042755344 3.3508064516129 3.34325744308231 3.3343653250774 3.32593619972261 3.31486146095718 3.26812428078251 3.16101694915254 3.03732809430255 2.89670932358318 2.77634961439589 2.67552334943639 2.57511380880121 2.49461593682699 2.41933287950987 2.35580038885288 2.27891156462585 2.21572104018913 2.14827391058291</v>
+        <v>2.84195402298851 2.90973871733967 2.94959677419355 2.97197898423818 2.9906976744186 2.99722607489598 3.00755667506297 3.0253164556962 3.01483050847458 3.01866404715128 2.98264840182648 2.92373607540703 2.84219001610306 2.75626423690205 2.65948275862069 2.56373551465576 2.48116883116883 2.38723667905824 2.30728241563055 2.22448979591837</v>
       </c>
     </row>
     <row r="61" spans="6:29" x14ac:dyDescent="0.2">
@@ -32272,6 +32285,9 @@
       <c r="AB106" t="s">
         <v>147</v>
       </c>
+      <c r="AC106" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="107" spans="6:29" x14ac:dyDescent="0.2">
       <c r="F107" s="4">
@@ -32330,6 +32346,9 @@
       <c r="AB107" t="s">
         <v>147</v>
       </c>
+      <c r="AC107" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="108" spans="6:29" x14ac:dyDescent="0.2">
       <c r="F108" s="4">
@@ -32388,6 +32407,9 @@
       <c r="AB108" t="s">
         <v>147</v>
       </c>
+      <c r="AC108" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="109" spans="6:29" x14ac:dyDescent="0.2">
       <c r="F109" s="4">
@@ -32445,6 +32467,9 @@
       </c>
       <c r="AB109" t="s">
         <v>147</v>
+      </c>
+      <c r="AC109" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="110" spans="6:29" x14ac:dyDescent="0.2">
@@ -41114,7 +41139,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E89DAA0-8AA0-F247-8626-C062B2B43DC4}">
   <dimension ref="A1:X130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>

</xml_diff>